<commit_message>
Added citation table post
</commit_message>
<xml_diff>
--- a/data/Intro_survey_clean.xlsx
+++ b/data/Intro_survey_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rzc782/Dropbox/Work/R/Dataviz-Blog-Quarto/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C122266-1C9D-8E44-89F8-B0216E1749C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA858224-7C8A-4B43-A9AE-AB789A19C2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="500" windowWidth="34560" windowHeight="19720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -866,12 +866,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1208,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7303,8 +7306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0679C115-276F-D940-A2C8-4B2C08DF1E2A}">
   <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7493,11 +7496,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>72</v>
       </c>
     </row>
@@ -7557,11 +7560,11 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -7727,5 +7730,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>